<commit_message>
Added steel unit data from IEAGHG2013
</commit_message>
<xml_diff>
--- a/data/steel/SteelUnits_Variables.xlsx
+++ b/data/steel/SteelUnits_Variables.xlsx
@@ -1,46 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\steel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C6F935-C98F-7E42-B66F-A1B333A579D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="4725" windowWidth="25200" windowHeight="12435" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="9400" yWindow="560" windowWidth="17440" windowHeight="16180" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lime Kiln" sheetId="1" r:id="rId1"/>
     <sheet name="Coke Oven" sheetId="2" r:id="rId2"/>
     <sheet name="Sinter Plant" sheetId="3" r:id="rId3"/>
     <sheet name="Blast Furnace" sheetId="5" r:id="rId4"/>
-    <sheet name="Power Plant" sheetId="4" r:id="rId5"/>
-    <sheet name="Heat Recovery" sheetId="9" r:id="rId6"/>
-    <sheet name="BOF Steelmaking" sheetId="6" r:id="rId7"/>
-    <sheet name="Rolling" sheetId="7" r:id="rId8"/>
-    <sheet name="Air Seperation" sheetId="8" r:id="rId9"/>
-    <sheet name="Electric Arc Furnace" sheetId="11" r:id="rId10"/>
-    <sheet name="CO2 Capture" sheetId="12" r:id="rId11"/>
+    <sheet name="BOF Steelmaking" sheetId="6" r:id="rId5"/>
+    <sheet name="Ladle Metallurgy" sheetId="7" r:id="rId6"/>
+    <sheet name="Forming" sheetId="13" r:id="rId7"/>
+    <sheet name="Reference Values" sheetId="14" r:id="rId8"/>
+    <sheet name="Power Plant" sheetId="4" r:id="rId9"/>
+    <sheet name="Heat Recovery" sheetId="9" r:id="rId10"/>
+    <sheet name="Air Seperation" sheetId="8" r:id="rId11"/>
+    <sheet name="Electric Arc Furnace" sheetId="11" r:id="rId12"/>
+    <sheet name="CO2 Capture" sheetId="12" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samantha Tanzer - TBM</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
@@ -49,36 +53,54 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Table D1, pg 95 of the PDF</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Table D1, pg 95 of the PDF</t>
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Samantha Tanzer - TBM:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-COG, BFG, and Steam consumption, multplied by their respective heat content (pg c-13 to c-15) and converted to GJ</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>COG, BFG, and Steam consumption, multplied by their respective heat content (pg c-13 to c-15) and converted to GJ</t>
         </r>
       </text>
     </comment>
@@ -87,18 +109,18 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samantha Tanzer - TBM</author>
   </authors>
   <commentList>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -107,12 +129,528 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-COG + BFG + Steam Consumption from Table D-5</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>COG + BFG + Steam Consumption from Table D-5</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{8C24CC26-976E-A54B-A77B-3C3E41B0C739}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[(hot metal + scrap in) - liquid steel out] / hot metal in</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{14574FDC-7B1A-1F4F-9398-11418352A89A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>scrap / total metal in</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{47F1E4A8-0F44-3F48-A134-4DF602EA31E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[Nm3 BOF gas * (mj/Nm3) + kg steam * (mj/kg)] / 1000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{850C9328-3FFA-474C-9561-EAD266EA8ECC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lime + Burnt Dolomite</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{6E6ADCFC-FB5E-1D4A-8346-4C1CD99FF3A4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> (g/mol * mol/nM3 / g/kg) / kg/t  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{392F1A16-A245-3A46-AFAA-E2918C3B2CA9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Page numbers are those of PDF</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{78321E9A-6BCC-5546-A40C-84F68D8AE3B5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nm3 /kg * MJ/Nm3 = MJ/kg = GJ/t
+using: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1000 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">/ g/Nm3 = Nm3/kg </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>g/mol * mol/Nm3 = g/Nm3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{CA660664-4C5B-5341-AD1F-59F7E6F42A9C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nm3 /kg * MJ/Nm3 = MJ/kg = GJ/t
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">using: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1000 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">/ g/Nm3 = Nm3/kg </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>g/mol * mol/Nm3 = g/Nm3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{49295FB3-30D1-1142-AF52-72D7563F1579}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nm3 /kg * MJ/Nm3 = MJ/kg = GJ/t
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">using: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1000 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">/ g/Nm3 = Nm3/kg </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>g/mol * mol/Nm3 = g/Nm3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{06459B3F-9073-B64D-8001-6DD0C93C0FB5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>9 bar, 175C</t>
         </r>
       </text>
     </comment>
@@ -121,7 +659,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="147">
   <si>
     <t>Electricity Demand</t>
   </si>
@@ -183,24 +721,12 @@
     <t>MJ Electricity Out / MJ Fuel In</t>
   </si>
   <si>
-    <t>% C</t>
-  </si>
-  <si>
     <t>MJ Usable Heat / MJ Waste Heat</t>
   </si>
   <si>
     <t>Scrap Fraction of Steel</t>
   </si>
   <si>
-    <t>% scrap</t>
-  </si>
-  <si>
-    <t>Steam Production</t>
-  </si>
-  <si>
-    <t>MJ / t Hot Metal</t>
-  </si>
-  <si>
     <t>Process CO2</t>
   </si>
   <si>
@@ -249,9 +775,6 @@
     <t>MJ Electricity / t Hot Rolled Coil</t>
   </si>
   <si>
-    <t>MJ / t hot rolled coil</t>
-  </si>
-  <si>
     <t>EU-BAT-median</t>
   </si>
   <si>
@@ -369,20 +892,225 @@
     <t>Fe in Hot metal</t>
   </si>
   <si>
-    <t>remainder is assumed to be carboon</t>
-  </si>
-  <si>
     <t>Iron Ore Demand</t>
   </si>
   <si>
     <t>CaCO3 demand</t>
+  </si>
+  <si>
+    <t>Flux Demand</t>
+  </si>
+  <si>
+    <t>t / t liquid steel</t>
+  </si>
+  <si>
+    <t>t scrap / t metal in</t>
+  </si>
+  <si>
+    <t>Metal Loss</t>
+  </si>
+  <si>
+    <t>t loss / t metal in</t>
+  </si>
+  <si>
+    <t>t C /  t hot metal</t>
+  </si>
+  <si>
+    <t>t CaO / t flux</t>
+  </si>
+  <si>
+    <t>Lime in Flux</t>
+  </si>
+  <si>
+    <t>Oxygen Demand</t>
+  </si>
+  <si>
+    <t>t O2 / t liquid steel</t>
+  </si>
+  <si>
+    <t>t steel lost / t steel in</t>
+  </si>
+  <si>
+    <t>Steel Loss</t>
+  </si>
+  <si>
+    <t>t O2 / t steel out</t>
+  </si>
+  <si>
+    <t>t flux / t steel out</t>
+  </si>
+  <si>
+    <t>t CaO / t Flux</t>
+  </si>
+  <si>
+    <t>GJ / t Hot Metal</t>
+  </si>
+  <si>
+    <t>Heat Export</t>
+  </si>
+  <si>
+    <t>Burnt Dolomite</t>
+  </si>
+  <si>
+    <t>Hot Rolled Coil</t>
+  </si>
+  <si>
+    <t>Liquid Steel</t>
+  </si>
+  <si>
+    <t>Hot Metal</t>
+  </si>
+  <si>
+    <t>Sinter</t>
+  </si>
+  <si>
+    <t>CaO</t>
+  </si>
+  <si>
+    <t>C (t/t)</t>
+  </si>
+  <si>
+    <t>Fe (t/t)</t>
+  </si>
+  <si>
+    <t>Composition of Products</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>BOFG</t>
+  </si>
+  <si>
+    <t>BFG</t>
+  </si>
+  <si>
+    <t>COG</t>
+  </si>
+  <si>
+    <t>GJ/t</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Molar Mass</t>
+  </si>
+  <si>
+    <t>g/mol</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>HCs (BTX)</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>CONSTANTS</t>
+  </si>
+  <si>
+    <t>IEAGHG 2013 (Steel)</t>
+  </si>
+  <si>
+    <t>Conversions</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Table C-24, p87</t>
+  </si>
+  <si>
+    <t>Table C-23, p 86</t>
+  </si>
+  <si>
+    <t>p88</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>kWh in MJ</t>
+  </si>
+  <si>
+    <t>mol in Nm3</t>
+  </si>
+  <si>
+    <t>t / Nm3</t>
+  </si>
+  <si>
+    <t>Properties of of Produced Gases</t>
+  </si>
+  <si>
+    <t>MJ/Nm3 (LHV)</t>
+  </si>
+  <si>
+    <t>Alloy Demand</t>
+  </si>
+  <si>
+    <t>t Alloy metals / t steel out</t>
+  </si>
+  <si>
+    <t>t scrap / t steel out</t>
+  </si>
+  <si>
+    <t>GJ electricity / t steel</t>
+  </si>
+  <si>
+    <t>GJ heat / GJ steel</t>
+  </si>
+  <si>
+    <t>t lost / t stee out</t>
+  </si>
+  <si>
+    <t>Steel loss</t>
+  </si>
+  <si>
+    <t>remainder is assumed to be carbon</t>
+  </si>
+  <si>
+    <t>Scrap Demand</t>
+  </si>
+  <si>
+    <t>kWh in GJ</t>
+  </si>
+  <si>
+    <t>GJ Electricity / t steel out</t>
+  </si>
+  <si>
+    <t>GJ heat / t steel out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="173" formatCode="0.00000"/>
+    <numFmt numFmtId="174" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,37 +1158,63 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -471,7 +1225,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -479,11 +1233,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -492,7 +1326,46 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,6 +1459,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -621,6 +1511,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -796,24 +1703,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -827,7 +1734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -841,7 +1748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -853,62 +1760,179 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>0.12</v>
@@ -917,9 +1941,9 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>7.0000000000000007E-2</v>
@@ -933,29 +1957,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -964,36 +1988,36 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>0.9</v>
@@ -1005,12 +2029,12 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>0.872</v>
@@ -1022,7 +2046,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1031,30 +2055,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>10</v>
@@ -1066,37 +2090,37 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1105,7 +2129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1119,7 +2143,7 @@
       </c>
       <c r="E4">
         <f>E5</f>
-        <v>5.7313459999999994</v>
+        <v>3.3926379999999998</v>
       </c>
       <c r="F4">
         <v>0.88</v>
@@ -1133,12 +2157,12 @@
         <v>charcoal</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
       </c>
       <c r="C5">
         <f>1/1.2852</f>
@@ -1149,8 +2173,8 @@
         <v>0.126</v>
       </c>
       <c r="E5">
-        <f>(112.6*17.33+450.4*7.47+150*2.77)/1000</f>
-        <v>5.7313459999999994</v>
+        <f>(112.6*'Reference Values'!F4+450.4*'Reference Values'!F5+150*'Reference Values'!F7)/1000</f>
+        <v>3.3926379999999998</v>
       </c>
       <c r="F5">
         <v>0.88</v>
@@ -1159,7 +2183,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1170,25 +2194,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="16.1640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1196,66 +2220,66 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2"/>
       <c r="F3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1296,9 +2320,9 @@
         <v>0.69769999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>9.4E-2</v>
@@ -1317,10 +2341,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H5">
-        <f>17.33*4.2/1000</f>
+        <f>'Reference Values'!F4*4.2/1000</f>
         <v>7.2786000000000003E-2</v>
       </c>
       <c r="I5">
@@ -1337,48 +2361,48 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="6" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="6" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I1" t="s">
         <v>16</v>
@@ -1390,19 +2414,19 @@
         <v>0</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="M1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="N1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" t="s">
         <v>78</v>
       </c>
-      <c r="O1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1416,7 +2440,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -1425,33 +2449,33 @@
         <v>18</v>
       </c>
       <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
         <v>74</v>
       </c>
-      <c r="K2" t="s">
-        <v>74</v>
-      </c>
-      <c r="L2" t="s">
-        <v>76</v>
-      </c>
-      <c r="M2" t="s">
-        <v>79</v>
-      </c>
       <c r="N2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="O2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +2513,7 @@
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>3.7508219999999999</v>
+        <v>1.6824780000000001</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
@@ -1512,9 +2536,9 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>0.95</v>
@@ -1532,7 +2556,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H5">
         <f>0.1253+0.3518</f>
@@ -1542,8 +2566,8 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="J5">
-        <f>(8.6*17.33+479.2*7.47+8*2.77)/1000</f>
-        <v>3.7508219999999999</v>
+        <f>(8.6*'Reference Values'!F4+479.2*'Reference Values'!F5+8*'Reference Values'!F7)/1000</f>
+        <v>1.6824780000000001</v>
       </c>
       <c r="K5">
         <f>(98.8+4.9)*3.6/1000</f>
@@ -1570,102 +2594,323 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="B4">
+        <f>B5</f>
+        <v>8.7424712538784408E-2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:I4" si="0">C5</f>
+        <v>0.17338930461763097</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>4.7E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.80660799999999999</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>7.569999999999999E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0.91360634081902259</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>7.4236530739716242E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <f>((900.8+116.9+73.1+5)-1000)/(900.8+116.9+73.1+5)</f>
+        <v>8.7424712538784408E-2</v>
+      </c>
+      <c r="C5">
+        <f>(116.9+73.1)/(900.8+116.9+73.1+5)</f>
+        <v>0.17338930461763097</v>
+      </c>
+      <c r="D5">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E5">
+        <f>20*3.6/1000</f>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F5">
+        <f>(81.8*'Reference Values'!F6+70.6*'Reference Values'!I7)/1000</f>
+        <v>0.80660799999999999</v>
+      </c>
+      <c r="G5">
+        <f>0.0648+0.0109</f>
+        <v>7.569999999999999E-2</v>
+      </c>
+      <c r="H5">
+        <f>(0.0648+0.0109*'Reference Values'!H15)/(0.0648+0.0109)</f>
+        <v>0.91360634081902259</v>
+      </c>
+      <c r="I5">
+        <f>52*'Reference Values'!C12</f>
+        <v>7.4236530739716242E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="B4" s="5">
+        <f>B5</f>
+        <v>0.01</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" ref="C4:I4" si="0">C5</f>
+        <v>1.55E-2</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
+        <v>1.5597E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="0"/>
+        <v>2.9980137414116173E-3</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <v>1.55E-2</v>
+      </c>
+      <c r="D5">
+        <v>1E-3</v>
+      </c>
+      <c r="E5">
+        <f>25*'Reference Values'!B17/1000</f>
+        <v>0.09</v>
+      </c>
+      <c r="F5">
+        <f>0.9*'Reference Values'!F4/1000</f>
+        <v>1.5597E-2</v>
+      </c>
+      <c r="G5">
+        <f>2.1*'Reference Values'!C12</f>
+        <v>2.9980137414116173E-3</v>
+      </c>
+      <c r="H5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1674,186 +2919,531 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3781CE4-7743-9846-9145-8878AB6BF356}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>145</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="B4">
+        <f>B5</f>
+        <v>8.629999999999996E-2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:E4" si="0">C5</f>
+        <v>0.41832000000000003</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1.4799819999999997</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>6.8657369929508343E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <f>((1086.3-1052.6)+(1052.6-1000))/1000</f>
+        <v>8.629999999999996E-2</v>
+      </c>
+      <c r="C5">
+        <f>(10.9+105.3)*'Reference Values'!B18</f>
+        <v>0.41832000000000003</v>
+      </c>
+      <c r="D5">
+        <f>(1.1+84.3)*'Reference Values'!F4/1000</f>
+        <v>1.4799819999999997</v>
+      </c>
+      <c r="E5">
+        <f>(2.1*(1.052/1)+2.6)*'Reference Values'!C12</f>
+        <v>6.8657369929508343E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05A383-1270-574C-99EE-D090571D54CA}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="19"/>
+      <c r="B3" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="41">
+        <v>12</v>
+      </c>
+      <c r="C4" s="45">
+        <f>(B4*$B$19)/1000/1000</f>
+        <v>5.3537967341839917E-4</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="21">
+        <v>17.329999999999998</v>
+      </c>
+      <c r="G4" s="27">
+        <f>(0.2304*B5)+(0.5953*B8)+(0.0384*B6)+(0.0096*B7)+(0.0576*B11)+(0.0019*B12)+(0.0398*B9)+(0.0269*B10)</f>
+        <v>11.269190558666665</v>
+      </c>
+      <c r="H4" s="25">
+        <f>(G4*$B$19)/1000/1000</f>
+        <v>5.0277463008238893E-4</v>
+      </c>
+      <c r="I4" s="28">
+        <f>1000/(G4*$B$19) *F4</f>
+        <v>34.468724082518165</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="41">
+        <v>16.042459999999998</v>
+      </c>
+      <c r="C5" s="45">
+        <f t="shared" ref="C5:C12" si="0">(B5*$B$19)/1000/1000</f>
+        <v>7.1573391630231102E-4</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="21">
+        <v>3.2</v>
+      </c>
+      <c r="G5" s="27">
+        <f>0.0363*B8+0.2234*B6+0.221*B7+0.4877*B11+0.0315*B9</f>
+        <v>30.286348783999998</v>
+      </c>
+      <c r="H5" s="25">
+        <f>(G5*$B$19)/1000/1000</f>
+        <v>1.3512246267511374E-3</v>
+      </c>
+      <c r="I5" s="28">
+        <f>1000/(G5*$B$19) *F5</f>
+        <v>2.3682220828775362</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="41">
+        <v>28.010100000000001</v>
+      </c>
+      <c r="C6" s="45">
+        <f t="shared" si="0"/>
+        <v>1.2496698492013921E-3</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="21">
+        <v>7.47</v>
+      </c>
+      <c r="G6" s="27">
+        <f>0.0264*B8+0.5692*B6+0.1444*B7*0.1383*B11+0.1216*B9</f>
+        <v>42.807996159159202</v>
+      </c>
+      <c r="H6" s="25">
+        <f>(G6*$B$19)/1000/1000</f>
+        <v>1.9098775836155618E-3</v>
+      </c>
+      <c r="I6" s="28">
+        <f>1000/(G6*$B$19) *F6</f>
+        <v>3.9112454453016037</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="41">
+        <v>44.009500000000003</v>
+      </c>
+      <c r="C7" s="45">
+        <f t="shared" si="0"/>
+        <v>1.963482644775587E-3</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="26">
+        <f>C9</f>
+        <v>8.0375122691175155E-4</v>
+      </c>
+      <c r="I7" s="30">
+        <v>2.77</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="41">
+        <v>2.0158800000000001</v>
+      </c>
+      <c r="C8" s="45">
+        <f t="shared" si="0"/>
+        <v>8.9938431337556905E-5</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="41">
+        <v>18.015280000000001</v>
+      </c>
+      <c r="C9" s="45">
+        <f t="shared" si="0"/>
+        <v>8.0375122691175155E-4</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="41">
+        <f>(78.12+92.15+106.7)/3</f>
+        <v>92.323333333333338</v>
+      </c>
+      <c r="C10" s="45">
+        <f t="shared" si="0"/>
+        <v>4.1190030040748338E-3</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="41">
+        <v>28.013400000000001</v>
+      </c>
+      <c r="C11" s="45">
+        <f t="shared" si="0"/>
+        <v>1.2498170786115822E-3</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0.57879999999999998</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="15">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="41">
+        <v>31.998799999999999</v>
+      </c>
+      <c r="C12" s="45">
+        <f t="shared" si="0"/>
+        <v>1.4276255911483892E-3</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.94240000000000002</v>
+      </c>
+      <c r="G12" s="14">
+        <v>4.65E-2</v>
+      </c>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="33"/>
+      <c r="E13" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="14">
+        <v>0.99909999999999999</v>
+      </c>
+      <c r="G13" s="14">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="E14" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0.98729999999999996</v>
+      </c>
+      <c r="G14" s="14">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="E15" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="19"/>
+      <c r="B16" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="42"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="32">
+        <v>3.6</v>
+      </c>
+      <c r="C17" s="41"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="31">
+        <f>B17/1000</f>
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="33">
+        <f>1/0.022414</f>
+        <v>44.614972784866602</v>
+      </c>
+      <c r="C19" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>